<commit_message>
Added description on README
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_presidents_comment.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_presidents_comment.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\workspace\exceltable\xlbean\src\test\java\com\xlbean\reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="presidents" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>谷川和也</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -134,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -149,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -164,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0">
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="177" formatCode="_-\$* #,##0.00_ ;_-\$* \-#,##0.00\ ;_-\$* &quot;-&quot;??_ ;_-@_ "/>
@@ -704,15 +704,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="テーブル4" displayName="テーブル4" ref="B6:G17" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B6:G17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="テーブル4" displayName="テーブル4" ref="B6:G17" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B6:G17" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Name" dataDxfId="5"/>
-    <tableColumn id="2" name="Date of birth" dataDxfId="4"/>
-    <tableColumn id="3" name="State of birth" dataDxfId="3"/>
-    <tableColumn id="4" name="In office from" dataDxfId="2"/>
-    <tableColumn id="5" name="In office to" dataDxfId="1"/>
-    <tableColumn id="6" name="# of days _x000a_in office" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Date of birth" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="State of birth" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="In office from" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="In office to" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="# of days _x000a_in office" dataDxfId="0">
       <calculatedColumnFormula>テーブル4[[#This Row],[In office to]]-テーブル4[[#This Row],[In office from]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1016,18 +1016,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="2.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.58203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
     <col min="5" max="6" width="12.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" style="1" customWidth="1"/>

</xml_diff>